<commit_message>
Make parser case insensitive; add direction synonyms
</commit_message>
<xml_diff>
--- a/proj/Demongeon Product Backlog.xlsx
+++ b/proj/Demongeon Product Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Partition</t>
   </si>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,6 +946,9 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C13" s="2">
         <v>3</v>
       </c>
@@ -1049,6 +1052,9 @@
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C17" s="2">
         <v>3</v>

</xml_diff>

<commit_message>
Implement Death subclass of Situation
Now you can die in an object-oriented manner.  Should have Hero class
raise a LifeException instead.
</commit_message>
<xml_diff>
--- a/proj/Demongeon Product Backlog.xlsx
+++ b/proj/Demongeon Product Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
   <si>
     <t>Partition</t>
   </si>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,116 +653,119 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
+      <c r="B3" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -771,24 +774,24 @@
         <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -797,212 +800,215 @@
         <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>27</v>
@@ -1011,76 +1017,73 @@
         <v>23</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2">
-        <v>-1</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="H16" s="2" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -1089,71 +1092,71 @@
         <v>55</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C20" s="2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1177,6 +1180,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I24">
+    <sortCondition descending="1" ref="C2:C24"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement Victory subclass of Situation
</commit_message>
<xml_diff>
--- a/proj/Demongeon Product Backlog.xlsx
+++ b/proj/Demongeon Product Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
   <si>
     <t>Partition</t>
   </si>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,6 +848,9 @@
       <c r="A9" s="2">
         <v>14</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C9" s="2">
         <v>2</v>
       </c>

</xml_diff>